<commit_message>
Update graph and log scale
</commit_message>
<xml_diff>
--- a/Misure Tot.xlsx
+++ b/Misure Tot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\uni\Bicocca\Magistrale\1 anno\Metodi del calcolo scientifico\Progetto\1\TEMPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2984680A-6911-4D6C-8682-D29F29D580AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB950E3-62BA-446C-9E8F-1F444054A735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="49">
   <si>
     <t>MATRICE</t>
   </si>
@@ -143,14 +143,54 @@
   <si>
     <t>Err Ubuntu</t>
   </si>
+  <si>
+    <t>MATLAB (s)</t>
+  </si>
+  <si>
+    <t>R (s)</t>
+  </si>
+  <si>
+    <t>Python (s)</t>
+  </si>
+  <si>
+    <t>C++ (s)</t>
+  </si>
+  <si>
+    <t>Fake, creato solo per il grafico</t>
+  </si>
+  <si>
+    <t>MATLAB (MB)</t>
+  </si>
+  <si>
+    <t>Python (MB)</t>
+  </si>
+  <si>
+    <t>C++ (MB)</t>
+  </si>
+  <si>
+    <t>R (MB)</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R </t>
+  </si>
+  <si>
+    <t>MATLAB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000000000000000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000000000000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -175,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -300,11 +340,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -342,6 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -349,6 +442,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -360,15 +462,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -378,7 +471,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1955,6 +2068,1892 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="546840367"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$E$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C++ (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.2777777777777778E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US">
+                        <a:solidFill>
+                          <a:srgbClr val="FF0000"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>FAKE</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-78F6-4A39-B5D6-6002FAC1D207}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$E$44:$E$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>867</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11107.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21938</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-78F6-4A39-B5D6-6002FAC1D207}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$F$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Python (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$F$44:$F$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.96499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.59</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2109999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.376999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-78F6-4A39-B5D6-6002FAC1D207}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$G$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$G$44:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.3906400000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.41</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61.929000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>88.35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.499000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6359999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1871.466075</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-78F6-4A39-B5D6-6002FAC1D207}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$H$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MATLAB (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$H$44:$H$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.145652</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.419437</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.119775</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.1559869999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.59745</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8173779999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47.19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>403.65339999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-78F6-4A39-B5D6-6002FAC1D207}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="45991519"/>
+        <c:axId val="45984447"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="45991519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="45984447"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="45984447"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="45991519"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>RAM</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" baseline="0"/>
+              <a:t> Peak</a:t>
+            </a:r>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$E$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C++ (MB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5555555555555552E-2"/>
+                  <c:y val="-2.3148148148148147E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US">
+                        <a:solidFill>
+                          <a:srgbClr val="FF0000"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>FAKE</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-9101-4100-80B7-17D12A685F5F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$E$58:$E$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2335</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>752</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3904.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7057</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9101-4100-80B7-17D12A685F5F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$F$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Python (MB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$F$58:$F$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>176.12800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>258.048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>536.57600000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1540.096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>860.16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>901.12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5013.5039999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9101-4100-80B7-17D12A685F5F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$G$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R (MB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$G$58:$G$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>21.86308</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.548802999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>163.57148000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1988.8832640000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>274.94207999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85.275335999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1418.6064799999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9101-4100-80B7-17D12A685F5F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$H$57</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MATLAB (MB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$H$58:$H$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>79.861000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.525000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>402.24799999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1584.64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1853.4390000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>506.88</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6261.2280000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10821.608249999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9101-4100-80B7-17D12A685F5F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1956560271"/>
+        <c:axId val="1956578159"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1956560271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1956578159"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1956578159"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1956560271"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Error</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$E$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.8888888888888994E-2"/>
+                  <c:y val="4.1666666666666664E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US">
+                        <a:solidFill>
+                          <a:srgbClr val="FF0000"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>FAKE</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-27A3-4ABD-8599-7F9251FBCA06}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$E$69:$E$76</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000000000000E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9.0404699999999995E-13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1203000000000001E-11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7767700000000003E-15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.2565100000000004E-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2928900000000002E-14</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>2.701557146445E-8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4031100000000001E-8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-27A3-4ABD-8599-7F9251FBCA06}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$F$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Python </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$F$69:$F$76</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000000000000E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.5421964438401398E-13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.66696719991457E-11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.4898639616557602E-15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0146065635240301E-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.3564967382118697E-14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.32264230605292E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.1640007644011202E-10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-27A3-4ABD-8599-7F9251FBCA06}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$G$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$G$69:$G$76</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000000000000E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7.7931218627444002E-13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0046500697320201E-11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0191779216228101E-14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4129522772949801E-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2939988823147899E-14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6267756992300603E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.50249542234088E-8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-27A3-4ABD-8599-7F9251FBCA06}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$H$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MATLAB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$H$69:$H$76</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000000000000E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.80985793527588E-15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4303331893609901E-11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3890062432155104E-16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5748490751662501E-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3311170240323398E-14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.12101483800396E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.5005772771062001E-11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.4255806455859999E-14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-27A3-4ABD-8599-7F9251FBCA06}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1958240511"/>
+        <c:axId val="1958240927"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1958240511"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1958240927"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1958240927"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000000000000000E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1958240511"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5479,6 +7478,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -7348,6 +9467,1554 @@
 </file>
 
 <file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12425,6 +16092,114 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Grafico 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76CB0CCC-72FF-42E5-BF8B-E5E592A8A048}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Grafico 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{582878B3-A8E8-4863-B33E-63684F7364A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>119062</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>280987</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="Grafico 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E69BB399-35FE-41A4-A04F-62D2A2D1D00A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -12691,10 +16466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L40"/>
+  <dimension ref="B1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O64" sqref="O64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12715,18 +16490,18 @@
       <c r="B1" s="16"/>
       <c r="C1" s="17"/>
       <c r="D1" s="18"/>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="43" t="s">
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="45"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="43"/>
     </row>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
@@ -12949,14 +16724,14 @@
       <c r="D8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="46"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="48"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="49"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -13003,31 +16778,31 @@
       <c r="D10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="46"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="48"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="49"/>
     </row>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="37" t="s">
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="40"/>
     </row>
     <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
@@ -13326,31 +17101,31 @@
       <c r="D20" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="42"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="46"/>
     </row>
     <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="16"/>
       <c r="C21" s="17"/>
       <c r="D21" s="18"/>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="43" t="s">
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="45"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="43"/>
     </row>
     <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
@@ -13656,10 +17431,10 @@
       <c r="D30" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E30" s="40"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="42"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="46"/>
       <c r="I30" s="34">
         <v>19.13</v>
       </c>
@@ -13671,18 +17446,18 @@
       <c r="B31" s="10"/>
       <c r="C31" s="11"/>
       <c r="D31" s="12"/>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="37" t="s">
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="40"/>
     </row>
     <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
@@ -13856,7 +17631,7 @@
       <c r="I36" s="1">
         <v>0.23162430000000001</v>
       </c>
-      <c r="J36" s="49">
+      <c r="J36" s="37">
         <v>15.3186938</v>
       </c>
       <c r="K36" s="29">
@@ -14015,13 +17790,405 @@
         <v>11653.983249999999</v>
       </c>
     </row>
+    <row r="42" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E43" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F43" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H43" s="50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E44" s="55">
+        <v>73</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="G44" s="11">
+        <v>1.3906400000000001</v>
+      </c>
+      <c r="H44" s="51">
+        <v>0.145652</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E45" s="51">
+        <v>38</v>
+      </c>
+      <c r="F45" s="3">
+        <v>1</v>
+      </c>
+      <c r="G45" s="2">
+        <v>17.41</v>
+      </c>
+      <c r="H45" s="51">
+        <v>0.419437</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E46" s="51">
+        <v>222</v>
+      </c>
+      <c r="F46" s="3">
+        <v>5.38</v>
+      </c>
+      <c r="G46" s="2">
+        <v>61.929000000000002</v>
+      </c>
+      <c r="H46" s="51">
+        <v>1.119775</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E47" s="51">
+        <v>867</v>
+      </c>
+      <c r="F47" s="21">
+        <v>1.59</v>
+      </c>
+      <c r="G47" s="19">
+        <v>88.35</v>
+      </c>
+      <c r="H47" s="51">
+        <v>8.1559869999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E48" s="51">
+        <v>277</v>
+      </c>
+      <c r="F48" s="21">
+        <v>3.6</v>
+      </c>
+      <c r="G48" s="2">
+        <v>15.499000000000001</v>
+      </c>
+      <c r="H48" s="51">
+        <v>1.59745</v>
+      </c>
+    </row>
+    <row r="49" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" s="56">
+        <f>(277+21938)/2</f>
+        <v>11107.5</v>
+      </c>
+      <c r="F49" s="6">
+        <v>3.2109999999999999</v>
+      </c>
+      <c r="G49" s="5">
+        <v>1.6359999999999999</v>
+      </c>
+      <c r="H49" s="52">
+        <v>1.8173779999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E50" s="51">
+        <v>21938</v>
+      </c>
+      <c r="F50" s="6">
+        <v>24.376999999999999</v>
+      </c>
+      <c r="G50" s="5">
+        <v>1871.466075</v>
+      </c>
+      <c r="H50" s="51">
+        <v>47.19</v>
+      </c>
+    </row>
+    <row r="51" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E51" s="53"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="54">
+        <v>403.65339999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E57" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="F57" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="G57" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H57" s="50" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E58" s="1">
+        <v>107</v>
+      </c>
+      <c r="F58" s="51">
+        <f>43*4.096</f>
+        <v>176.12800000000001</v>
+      </c>
+      <c r="G58" s="55">
+        <f xml:space="preserve"> 21863080/1000000</f>
+        <v>21.86308</v>
+      </c>
+      <c r="H58" s="3">
+        <f>638888/1000*0.125</f>
+        <v>79.861000000000004</v>
+      </c>
+    </row>
+    <row r="59" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E59" s="1">
+        <v>142</v>
+      </c>
+      <c r="F59" s="51">
+        <f>63*4.096</f>
+        <v>258.048</v>
+      </c>
+      <c r="G59" s="51">
+        <f>26548803/1000000</f>
+        <v>26.548802999999999</v>
+      </c>
+      <c r="H59" s="3">
+        <f>660200/1000*0.125</f>
+        <v>82.525000000000006</v>
+      </c>
+    </row>
+    <row r="60" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E60" s="1">
+        <v>413</v>
+      </c>
+      <c r="F60" s="51">
+        <f>131*4.096</f>
+        <v>536.57600000000002</v>
+      </c>
+      <c r="G60" s="51">
+        <f>163571480/1000000</f>
+        <v>163.57148000000001</v>
+      </c>
+      <c r="H60" s="3">
+        <f>3217984/1000*0.125</f>
+        <v>402.24799999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E61" s="1">
+        <v>2335</v>
+      </c>
+      <c r="F61" s="51">
+        <f>376*4.096</f>
+        <v>1540.096</v>
+      </c>
+      <c r="G61" s="51">
+        <f>1988883264/1000000</f>
+        <v>1988.8832640000001</v>
+      </c>
+      <c r="H61" s="3">
+        <f>12677120/1000*0.125</f>
+        <v>1584.64</v>
+      </c>
+    </row>
+    <row r="62" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E62" s="1">
+        <v>752</v>
+      </c>
+      <c r="F62" s="51">
+        <f>210*4.096</f>
+        <v>860.16</v>
+      </c>
+      <c r="G62" s="51">
+        <f>274942080/1000000</f>
+        <v>274.94207999999998</v>
+      </c>
+      <c r="H62" s="3">
+        <f>14827512/1000*0.125</f>
+        <v>1853.4390000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>40</v>
+      </c>
+      <c r="E63" s="59">
+        <f>(7057+752)/2</f>
+        <v>3904.5</v>
+      </c>
+      <c r="F63" s="52">
+        <f>220*4.096</f>
+        <v>901.12</v>
+      </c>
+      <c r="G63" s="52">
+        <f>85275336/1000000</f>
+        <v>85.275335999999996</v>
+      </c>
+      <c r="H63" s="6">
+        <f>4055040/1000*0.125</f>
+        <v>506.88</v>
+      </c>
+    </row>
+    <row r="64" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E64" s="1">
+        <v>7057</v>
+      </c>
+      <c r="F64" s="51">
+        <f>1224*4.096</f>
+        <v>5013.5039999999999</v>
+      </c>
+      <c r="G64" s="51">
+        <f>1418606480/1000000</f>
+        <v>1418.6064799999999</v>
+      </c>
+      <c r="H64" s="3">
+        <f>50089824/1000*0.125</f>
+        <v>6261.2280000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E65" s="57"/>
+      <c r="F65" s="53"/>
+      <c r="G65" s="58"/>
+      <c r="H65" s="9">
+        <f>86572866/1000*0.125</f>
+        <v>10821.608249999999</v>
+      </c>
+    </row>
+    <row r="67" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E68" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="F68" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="G68" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H68" s="50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E69" s="63">
+        <v>9.0404699999999995E-13</v>
+      </c>
+      <c r="F69" s="67">
+        <v>5.5421964438401398E-13</v>
+      </c>
+      <c r="G69" s="61">
+        <v>7.7931218627444002E-13</v>
+      </c>
+      <c r="H69" s="67">
+        <v>3.80985793527588E-15</v>
+      </c>
+    </row>
+    <row r="70" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E70" s="63">
+        <v>1.1203000000000001E-11</v>
+      </c>
+      <c r="F70" s="67">
+        <v>1.66696719991457E-11</v>
+      </c>
+      <c r="G70" s="60">
+        <v>3.0046500697320201E-11</v>
+      </c>
+      <c r="H70" s="67">
+        <v>2.4303331893609901E-11</v>
+      </c>
+    </row>
+    <row r="71" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E71" s="63">
+        <v>7.7767700000000003E-15</v>
+      </c>
+      <c r="F71" s="67">
+        <v>8.4898639616557602E-15</v>
+      </c>
+      <c r="G71" s="60">
+        <v>2.0191779216228101E-14</v>
+      </c>
+      <c r="H71" s="67">
+        <v>9.3890062432155104E-16</v>
+      </c>
+    </row>
+    <row r="72" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E72" s="63">
+        <v>6.2565100000000004E-12</v>
+      </c>
+      <c r="F72" s="67">
+        <v>3.0146065635240301E-12</v>
+      </c>
+      <c r="G72" s="60">
+        <v>2.4129522772949801E-12</v>
+      </c>
+      <c r="H72" s="67">
+        <v>3.5748490751662501E-12</v>
+      </c>
+    </row>
+    <row r="73" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E73" s="63">
+        <v>4.2928900000000002E-14</v>
+      </c>
+      <c r="F73" s="67">
+        <v>5.3564967382118697E-14</v>
+      </c>
+      <c r="G73" s="60">
+        <v>4.2939988823147899E-14</v>
+      </c>
+      <c r="H73" s="67">
+        <v>3.3311170240323398E-14</v>
+      </c>
+    </row>
+    <row r="74" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>40</v>
+      </c>
+      <c r="E74" s="64">
+        <f>(0.0000000540311+0.0000000000000429289)/2</f>
+        <v>2.701557146445E-8</v>
+      </c>
+      <c r="F74" s="68">
+        <v>1.32264230605292E-5</v>
+      </c>
+      <c r="G74" s="62">
+        <v>8.6267756992300603E-6</v>
+      </c>
+      <c r="H74" s="68">
+        <v>1.12101483800396E-5</v>
+      </c>
+    </row>
+    <row r="75" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E75" s="63">
+        <v>5.4031100000000001E-8</v>
+      </c>
+      <c r="F75" s="67">
+        <v>9.1640007644011202E-10</v>
+      </c>
+      <c r="G75" s="60">
+        <v>1.50249542234088E-8</v>
+      </c>
+      <c r="H75" s="67">
+        <v>4.5005772771062001E-11</v>
+      </c>
+    </row>
+    <row r="76" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E76" s="65"/>
+      <c r="F76" s="69"/>
+      <c r="G76" s="66"/>
+      <c r="H76" s="70">
+        <v>7.4255806455859999E-14</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E31:H31"/>
-    <mergeCell ref="I31:L31"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="I21:L21"/>
-    <mergeCell ref="E30:H30"/>
     <mergeCell ref="E11:H11"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="E20:H20"/>
@@ -14032,6 +18199,11 @@
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="I8:L8"/>
     <mergeCell ref="I10:L10"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="I31:L31"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="E30:H30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>